<commit_message>
First attempt at matching started.
</commit_message>
<xml_diff>
--- a/Data/dartsdatabase/Players.xlsx
+++ b/Data/dartsdatabase/Players.xlsx
@@ -280,12 +280,12 @@
     <t>Michael Mansell</t>
   </si>
   <si>
+    <t>Kim Viljanen</t>
+  </si>
+  <si>
     <t>Luke Humphries</t>
   </si>
   <si>
-    <t>Kim Viljanen</t>
-  </si>
-  <si>
     <t>Berry van Peer</t>
   </si>
   <si>
@@ -331,12 +331,12 @@
     <t>Cameron Menzies</t>
   </si>
   <si>
+    <t>Andy Boulton</t>
+  </si>
+  <si>
     <t>Kirk Shepherd</t>
   </si>
   <si>
-    <t>Andy Boulton</t>
-  </si>
-  <si>
     <t>Ross Montgomery</t>
   </si>
   <si>
@@ -349,6 +349,9 @@
     <t>Jeff Smith</t>
   </si>
   <si>
+    <t>Michael Barnard</t>
+  </si>
+  <si>
     <t>Martin Phillips</t>
   </si>
   <si>
@@ -358,12 +361,12 @@
     <t>Darius Labanauskas</t>
   </si>
   <si>
+    <t>Diogo Portela</t>
+  </si>
+  <si>
     <t>Chris Quantock</t>
   </si>
   <si>
-    <t>Diogo Portela</t>
-  </si>
-  <si>
     <t>Paul Hogan</t>
   </si>
   <si>
@@ -385,27 +388,27 @@
     <t>Vincent Kamphuis</t>
   </si>
   <si>
-    <t>Michael Barnard</t>
-  </si>
-  <si>
     <t>Peter Machin</t>
   </si>
   <si>
+    <t>Marko Kantele</t>
+  </si>
+  <si>
     <t>Richard Veenstra</t>
   </si>
   <si>
     <t>Scott Taylor</t>
   </si>
   <si>
-    <t>Marko Kantele</t>
-  </si>
-  <si>
     <t>Steve Hine</t>
   </si>
   <si>
     <t>Magnus Caris</t>
   </si>
   <si>
+    <t>Yordi Meeuwisse</t>
+  </si>
+  <si>
     <t>Wesley Harms</t>
   </si>
   <si>
@@ -415,9 +418,6 @@
     <t>Mark Walsh</t>
   </si>
   <si>
-    <t>Yordi Meeuwisse</t>
-  </si>
-  <si>
     <t>Hyun Chul Park</t>
   </si>
   <si>
@@ -427,6 +427,9 @@
     <t>Kevin Munch</t>
   </si>
   <si>
+    <t>Cody Harris</t>
+  </si>
+  <si>
     <t>Tengku Hadzali Shah</t>
   </si>
   <si>
@@ -466,27 +469,24 @@
     <t>Nick Kenny</t>
   </si>
   <si>
-    <t>Cody Harris</t>
+    <t>Stuart Kellett</t>
+  </si>
+  <si>
+    <t>Dennis Nilsson</t>
+  </si>
+  <si>
+    <t>John Bowles</t>
   </si>
   <si>
     <t>Ryan Joyce</t>
   </si>
   <si>
-    <t>John Bowles</t>
-  </si>
-  <si>
-    <t>Stuart Kellett</t>
-  </si>
-  <si>
     <t>Ritchie Edhouse</t>
   </si>
   <si>
     <t>Michael Unterbuchner</t>
   </si>
   <si>
-    <t>Dennis Nilsson</t>
-  </si>
-  <si>
     <t>Kenny Neyens</t>
   </si>
   <si>
@@ -496,15 +496,15 @@
     <t>Daniel Larsson</t>
   </si>
   <si>
+    <t>Matt Clark</t>
+  </si>
+  <si>
     <t>Andy Baetens</t>
   </si>
   <si>
     <t>Justin van Tergouw</t>
   </si>
   <si>
-    <t>Matt Clark</t>
-  </si>
-  <si>
     <t>Aden Kirk</t>
   </si>
   <si>
@@ -535,6 +535,9 @@
     <t>Luke Woodhouse</t>
   </si>
   <si>
+    <t>Harry Ward</t>
+  </si>
+  <si>
     <t>Alexander Oreshkin</t>
   </si>
   <si>
@@ -544,9 +547,6 @@
     <t>Willard Bruguier III</t>
   </si>
   <si>
-    <t>Harry Ward</t>
-  </si>
-  <si>
     <t>Maik Langendorf</t>
   </si>
   <si>
@@ -556,12 +556,12 @@
     <t>Jerry Hendriks</t>
   </si>
   <si>
+    <t>Wes Newton</t>
+  </si>
+  <si>
     <t>Kyle McKinstry</t>
   </si>
   <si>
-    <t>Wes Newton</t>
-  </si>
-  <si>
     <t>Dave Cameron</t>
   </si>
   <si>
@@ -586,13 +586,16 @@
     <t>Royden Lam</t>
   </si>
   <si>
+    <t>Jason Lowe</t>
+  </si>
+  <si>
+    <t>Jason Wilson</t>
+  </si>
+  <si>
     <t>Dawson Murschell</t>
   </si>
   <si>
-    <t>Jason Lowe</t>
-  </si>
-  <si>
-    <t>Jason Wilson</t>
+    <t>Barrie Bates</t>
   </si>
   <si>
     <t>Gary Robson</t>
@@ -601,24 +604,24 @@
     <t>Rene Eidams</t>
   </si>
   <si>
+    <t>Kevin Simm</t>
+  </si>
+  <si>
     <t>Stephen Burton</t>
   </si>
   <si>
     <t>Tony Newell</t>
   </si>
   <si>
-    <t>Kevin Simm</t>
-  </si>
-  <si>
-    <t>Barrie Bates</t>
+    <t>Matthew Dennant</t>
+  </si>
+  <si>
+    <t>Scott Dale</t>
   </si>
   <si>
     <t>Ross Twell</t>
   </si>
   <si>
-    <t>Scott Dale</t>
-  </si>
-  <si>
     <t>Mark Dudbridge</t>
   </si>
   <si>
@@ -628,15 +631,18 @@
     <t>Bernie Smith</t>
   </si>
   <si>
-    <t>Matthew Dennant</t>
-  </si>
-  <si>
     <t>Ryan Harrington</t>
   </si>
   <si>
+    <t>Michael Rasztovits</t>
+  </si>
+  <si>
     <t>Lee Evans</t>
   </si>
   <si>
+    <t>Nathan Rafferty</t>
+  </si>
+  <si>
     <t>Mark Barilli</t>
   </si>
   <si>
@@ -646,18 +652,15 @@
     <t>Andy Smith</t>
   </si>
   <si>
-    <t>Nathan Rafferty</t>
-  </si>
-  <si>
     <t>Tytus Kanik</t>
   </si>
   <si>
-    <t>Michael Rasztovits</t>
-  </si>
-  <si>
     <t>Daniel Day</t>
   </si>
   <si>
+    <t>Rusty Jake Rodriguez</t>
+  </si>
+  <si>
     <t>Sho Katsumi</t>
   </si>
   <si>
@@ -667,7 +670,7 @@
     <t>Robert Marijanovic</t>
   </si>
   <si>
-    <t>Rusty Jake Rodriguez</t>
+    <t>Adam Smith-Neale</t>
   </si>
   <si>
     <t>Brian Woods</t>
@@ -682,19 +685,19 @@
     <t>Gilbert Ulang</t>
   </si>
   <si>
-    <t>Adam Smith-Neale</t>
+    <t>Simon Preston</t>
   </si>
   <si>
     <t>Paul Harvey</t>
   </si>
   <si>
+    <t>Rhys Griffin</t>
+  </si>
+  <si>
     <t>Rob Hewson</t>
   </si>
   <si>
-    <t>Simon Preston</t>
-  </si>
-  <si>
-    <t>Rhys Griffin</t>
+    <t>Robert Rickwood</t>
   </si>
   <si>
     <t>Dyson Parody</t>
@@ -703,42 +706,45 @@
     <t>Steve Brown</t>
   </si>
   <si>
+    <t>Nathan Derry</t>
+  </si>
+  <si>
     <t>Aaron Dyer</t>
   </si>
   <si>
+    <t>Kevin Dowling</t>
+  </si>
+  <si>
+    <t>Jim Walker</t>
+  </si>
+  <si>
     <t>Matt Padgett</t>
   </si>
   <si>
     <t>Lourence Ilagan</t>
   </si>
   <si>
-    <t>Nathan Derry</t>
-  </si>
-  <si>
-    <t>Robert Rickwood</t>
-  </si>
-  <si>
-    <t>Kevin Dowling</t>
-  </si>
-  <si>
     <t>Nick Fullwell</t>
   </si>
   <si>
-    <t>Jim Walker</t>
+    <t>Jarred Cole</t>
+  </si>
+  <si>
+    <t>Dave Prins</t>
   </si>
   <si>
     <t>Ryan Palmer</t>
   </si>
   <si>
+    <t>Callum Loose</t>
+  </si>
+  <si>
     <t>Nigel Heydon</t>
   </si>
   <si>
     <t>Larry Butler</t>
   </si>
   <si>
-    <t>Callum Loose</t>
-  </si>
-  <si>
     <t>Kurt Parry</t>
   </si>
   <si>
@@ -748,9 +754,6 @@
     <t>Per Laursen</t>
   </si>
   <si>
-    <t>Jarred Cole</t>
-  </si>
-  <si>
     <t>Sven Groen</t>
   </si>
   <si>
@@ -760,6 +763,9 @@
     <t>Raymond Smith</t>
   </si>
   <si>
+    <t>Martin Atkins (Wigan)</t>
+  </si>
+  <si>
     <t>Justin Thompson</t>
   </si>
   <si>
@@ -775,9 +781,6 @@
     <t>Haruki Muramatsu</t>
   </si>
   <si>
-    <t>Dave Prins</t>
-  </si>
-  <si>
     <t>Mitsumasa Hoshino</t>
   </si>
   <si>
@@ -787,9 +790,15 @@
     <t>Prakash Jiwa</t>
   </si>
   <si>
+    <t>Martin Atkins</t>
+  </si>
+  <si>
     <t>Ricky Williams</t>
   </si>
   <si>
+    <t>Dennis Smith</t>
+  </si>
+  <si>
     <t>John Norman Jnr</t>
   </si>
   <si>
@@ -799,12 +808,6 @@
     <t>Bernd Roith</t>
   </si>
   <si>
-    <t>Dennis Smith</t>
-  </si>
-  <si>
-    <t>Martin Atkins</t>
-  </si>
-  <si>
     <t>Darin Young</t>
   </si>
   <si>
@@ -814,7 +817,7 @@
     <t>Ulf Ceder</t>
   </si>
   <si>
-    <t>Martin Atkins (Wigan)</t>
+    <t>Jason Cullen</t>
   </si>
   <si>
     <t>Daniel Jensen</t>
@@ -868,10 +871,13 @@
     <t>Alex Roy</t>
   </si>
   <si>
+    <t>Barry Lynn</t>
+  </si>
+  <si>
     <t>Dave Parletti</t>
   </si>
   <si>
-    <t>Jason Cullen</t>
+    <t>Jay Foreman</t>
   </si>
   <si>
     <t>Davy van Baelen</t>
@@ -883,9 +889,6 @@
     <t>Paul Milford</t>
   </si>
   <si>
-    <t>Jay Foreman</t>
-  </si>
-  <si>
     <t>Jose Perales</t>
   </si>
   <si>
@@ -901,9 +904,6 @@
     <t>David Evans</t>
   </si>
   <si>
-    <t>Barry Lynn</t>
-  </si>
-  <si>
     <t>Ioannis Selachoglou</t>
   </si>
   <si>
@@ -916,6 +916,9 @@
     <t>Bradley Brooks</t>
   </si>
   <si>
+    <t>Geert Nentjes</t>
+  </si>
+  <si>
     <t>Rhys Hayden</t>
   </si>
   <si>
@@ -934,18 +937,21 @@
     <t>Mark Wilson</t>
   </si>
   <si>
+    <t>Adam Huckvale</t>
+  </si>
+  <si>
+    <t>Mario Robbe</t>
+  </si>
+  <si>
+    <t>Yuanjun Liu</t>
+  </si>
+  <si>
     <t>Craig Caldwell</t>
   </si>
   <si>
     <t>Steffen Siepmann</t>
   </si>
   <si>
-    <t>Mario Robbe</t>
-  </si>
-  <si>
-    <t>Yuanjun Liu</t>
-  </si>
-  <si>
     <t>Howei Tsai</t>
   </si>
   <si>
@@ -967,24 +973,33 @@
     <t>Dennis Harbour</t>
   </si>
   <si>
-    <t>Geert Nentjes</t>
-  </si>
-  <si>
     <t>Stefan Stoyke</t>
   </si>
   <si>
     <t>Masumi Chino</t>
   </si>
   <si>
+    <t>Curtis Hammond</t>
+  </si>
+  <si>
     <t>Dan Read</t>
   </si>
   <si>
+    <t>Brett Claydon</t>
+  </si>
+  <si>
     <t>Rhys Mathewson</t>
   </si>
   <si>
+    <t>Jason Marriott</t>
+  </si>
+  <si>
     <t>Jamie Robinson</t>
   </si>
   <si>
+    <t>Ronnie Roberts</t>
+  </si>
+  <si>
     <t>Nandor Bezzeg</t>
   </si>
   <si>
@@ -994,9 +1009,6 @@
     <t>Sun Qiang</t>
   </si>
   <si>
-    <t>Ronnie Roberts</t>
-  </si>
-  <si>
     <t>Adam Rowe</t>
   </si>
   <si>
@@ -1006,21 +1018,12 @@
     <t>Dave Ladley</t>
   </si>
   <si>
-    <t>Jason Marriott</t>
-  </si>
-  <si>
     <t>Mark McGrath</t>
   </si>
   <si>
-    <t>Brett Claydon</t>
-  </si>
-  <si>
     <t>Yoeri Duijster</t>
   </si>
   <si>
-    <t>Curtis Hammond</t>
-  </si>
-  <si>
     <t>Craig Gilchrist</t>
   </si>
   <si>
@@ -1030,21 +1033,24 @@
     <t>Patrick Kovacs</t>
   </si>
   <si>
+    <t>Adrian Gray</t>
+  </si>
+  <si>
     <t>Roger Janssen</t>
   </si>
   <si>
     <t>Josh McCarthy</t>
   </si>
   <si>
+    <t>John Brown</t>
+  </si>
+  <si>
     <t>Robert Wagner</t>
   </si>
   <si>
     <t>Chris White</t>
   </si>
   <si>
-    <t>John Brown</t>
-  </si>
-  <si>
     <t>Christian Bunse</t>
   </si>
   <si>
@@ -1057,12 +1063,12 @@
     <t>Daniele Petri</t>
   </si>
   <si>
+    <t>Mike Zuydwijk</t>
+  </si>
+  <si>
     <t>Jyhan Artut</t>
   </si>
   <si>
-    <t>Mike Zuydwijk</t>
-  </si>
-  <si>
     <t>Thanawat Gaweenuntavong</t>
   </si>
   <si>
@@ -1093,9 +1099,6 @@
     <t>Alex Tagarao</t>
   </si>
   <si>
-    <t>Adrian Gray</t>
-  </si>
-  <si>
     <t>Yuji Eguchi</t>
   </si>
   <si>
@@ -1105,6 +1108,9 @@
     <t>Ryan de Vreede</t>
   </si>
   <si>
+    <t>Ryan Murray</t>
+  </si>
+  <si>
     <t>Kelvin Hart</t>
   </si>
   <si>
@@ -1114,7 +1120,7 @@
     <t>Fabian Herz</t>
   </si>
   <si>
-    <t>Ryan Murray</t>
+    <t>Thomas Lovely</t>
   </si>
   <si>
     <t>Jason Lovett</t>
@@ -1135,9 +1141,6 @@
     <t>John Goldie</t>
   </si>
   <si>
-    <t>Thomas Lovely</t>
-  </si>
-  <si>
     <t>Chris Harris</t>
   </si>
   <si>
@@ -1153,6 +1156,12 @@
     <t>Eddie Dootson</t>
   </si>
   <si>
+    <t>Mike Norton</t>
+  </si>
+  <si>
+    <t>Peter Mitchell</t>
+  </si>
+  <si>
     <t>Roxy James Rodriguez</t>
   </si>
   <si>
@@ -1162,27 +1171,21 @@
     <t>Trevor Burkhill</t>
   </si>
   <si>
+    <t>John Davey</t>
+  </si>
+  <si>
     <t>Tricia Wright</t>
   </si>
   <si>
-    <t>Peter Mitchell</t>
+    <t>Kevin Edwards</t>
   </si>
   <si>
     <t>Martin Marti</t>
   </si>
   <si>
-    <t>Mike Norton</t>
-  </si>
-  <si>
-    <t>John Davey</t>
-  </si>
-  <si>
     <t>Vincent van der Meer</t>
   </si>
   <si>
-    <t>Kevin Edwards</t>
-  </si>
-  <si>
     <t>Justin Smith</t>
   </si>
   <si>
@@ -1201,15 +1204,12 @@
     <t>Jake Jones</t>
   </si>
   <si>
+    <t>Lee Budgen</t>
+  </si>
+  <si>
     <t>Julio Barbero</t>
   </si>
   <si>
-    <t>Lee Budgen</t>
-  </si>
-  <si>
-    <t>Adam Huckvale</t>
-  </si>
-  <si>
     <t>Koha Kokiri</t>
   </si>
   <si>
@@ -1225,6 +1225,9 @@
     <t>Martyn Turner</t>
   </si>
   <si>
+    <t>John O Shea</t>
+  </si>
+  <si>
     <t>John Weber</t>
   </si>
   <si>
@@ -1246,7 +1249,7 @@
     <t>Jim Widmayer</t>
   </si>
   <si>
-    <t>John O Shea</t>
+    <t>Frantisek Humpula</t>
   </si>
   <si>
     <t>Jim Brown</t>
@@ -1282,9 +1285,6 @@
     <t>Paolo Nebrida</t>
   </si>
   <si>
-    <t>Frantisek Humpula</t>
-  </si>
-  <si>
     <t>Yuki Yamada</t>
   </si>
   <si>
@@ -1303,6 +1303,9 @@
     <t>Martijn Kleermaker</t>
   </si>
   <si>
+    <t>Michael Dawson</t>
+  </si>
+  <si>
     <t>Niels Zonneveld</t>
   </si>
   <si>
@@ -1315,7 +1318,7 @@
     <t>Joe Huffman</t>
   </si>
   <si>
-    <t>Michael Dawson</t>
+    <t>Greg Ritchie</t>
   </si>
   <si>
     <t>Sue Edwards</t>
@@ -1324,12 +1327,15 @@
     <t>Rachel Brooks</t>
   </si>
   <si>
+    <t>Ian Jones</t>
+  </si>
+  <si>
+    <t>Martin Thomas</t>
+  </si>
+  <si>
     <t>Ian Lever</t>
   </si>
   <si>
-    <t>Greg Ritchie</t>
-  </si>
-  <si>
     <t>Alan Soutar</t>
   </si>
   <si>
@@ -1366,9 +1372,6 @@
     <t>Edwin Torbjornsson</t>
   </si>
   <si>
-    <t>Ian Jones</t>
-  </si>
-  <si>
     <t>Silko Visser</t>
   </si>
   <si>
@@ -1381,7 +1384,7 @@
     <t>Dean Stewart</t>
   </si>
   <si>
-    <t>Martin Thomas</t>
+    <t>Kevin Garcia</t>
   </si>
   <si>
     <t>Andrew Townes</t>
@@ -1411,16 +1414,22 @@
     <t>Dean Finn</t>
   </si>
   <si>
+    <t>Ian Withers</t>
+  </si>
+  <si>
     <t>Kay Smeets</t>
   </si>
   <si>
     <t>Oliver Ferenc</t>
   </si>
   <si>
+    <t>Paul Phillips</t>
+  </si>
+  <si>
     <t>Darryl Pilgrim</t>
   </si>
   <si>
-    <t>Ian Withers</t>
+    <t>Tom Lonsdale</t>
   </si>
   <si>
     <t>Andy Parsons</t>
@@ -1432,12 +1441,12 @@
     <t>Colin Roelofs</t>
   </si>
   <si>
+    <t>Neil Duff</t>
+  </si>
+  <si>
     <t>Cyril Blot</t>
   </si>
   <si>
-    <t>Neil Duff</t>
-  </si>
-  <si>
     <t>Tony Alaentalo</t>
   </si>
   <si>
@@ -1465,9 +1474,15 @@
     <t>Sarah Roberts</t>
   </si>
   <si>
+    <t>Daniel Cole</t>
+  </si>
+  <si>
     <t>Alan Bell</t>
   </si>
   <si>
+    <t>Darren Beveridge</t>
+  </si>
+  <si>
     <t>Sam Hewson</t>
   </si>
   <si>
@@ -1513,21 +1528,6 @@
     <t>Kurt van de Rijck</t>
   </si>
   <si>
-    <t>Mike Symes</t>
-  </si>
-  <si>
-    <t>Carlo van Cleef</t>
-  </si>
-  <si>
-    <t>Francis Carragher</t>
-  </si>
-  <si>
-    <t>Philipp Ruckstuhl</t>
-  </si>
-  <si>
-    <t>Mick Baker</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -3094,6 +3094,9 @@
     <t>South Korea</t>
   </si>
   <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
     <t>Malaysia</t>
   </si>
   <si>
@@ -3106,9 +3109,6 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
@@ -3424,12 +3424,12 @@
     <t>PlayerDetails.aspx?playerKey=4083</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=95</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=11822</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=95</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=16990</t>
   </si>
   <si>
@@ -3475,12 +3475,12 @@
     <t>PlayerDetails.aspx?playerKey=5202</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=98</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=1492</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=98</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=199</t>
   </si>
   <si>
@@ -3493,6 +3493,9 @@
     <t>PlayerDetails.aspx?playerKey=4965</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=1399</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=194</t>
   </si>
   <si>
@@ -3502,12 +3505,12 @@
     <t>PlayerDetails.aspx?playerKey=4333</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=16009</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=13304</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=16009</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=180</t>
   </si>
   <si>
@@ -3529,27 +3532,27 @@
     <t>PlayerDetails.aspx?playerKey=9672</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=1399</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=2711</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=89</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=16652</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=11836</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=89</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=43</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=1868</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=8168</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=5875</t>
   </si>
   <si>
@@ -3559,9 +3562,6 @@
     <t>PlayerDetails.aspx?playerKey=15</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=8168</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=9094</t>
   </si>
   <si>
@@ -3571,6 +3571,9 @@
     <t>PlayerDetails.aspx?playerKey=1940</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=3944</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=2158</t>
   </si>
   <si>
@@ -3610,27 +3613,24 @@
     <t>PlayerDetails.aspx?playerKey=10013</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=3944</t>
+    <t>PlayerDetails.aspx?playerKey=2282</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=2494</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=9852</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=16151</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=9852</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=2282</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=17485</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=18178</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2494</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=13185</t>
   </si>
   <si>
@@ -3640,15 +3640,15 @@
     <t>PlayerDetails.aspx?playerKey=2381</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=37</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=10204</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=20142</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=37</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=10682</t>
   </si>
   <si>
@@ -3679,6 +3679,9 @@
     <t>PlayerDetails.aspx?playerKey=10621</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=16681</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=13428</t>
   </si>
   <si>
@@ -3688,9 +3691,6 @@
     <t>PlayerDetails.aspx?playerKey=23224</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=16681</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=2189</t>
   </si>
   <si>
@@ -3700,12 +3700,12 @@
     <t>PlayerDetails.aspx?playerKey=1000</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=24</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=17883</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=24</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=4960</t>
   </si>
   <si>
@@ -3730,13 +3730,16 @@
     <t>PlayerDetails.aspx?playerKey=5643</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=1489</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=13647</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=12485</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=1489</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=13647</t>
+    <t>PlayerDetails.aspx?playerKey=16</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=169</t>
@@ -3745,24 +3748,24 @@
     <t>PlayerDetails.aspx?playerKey=16615</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=2316</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=15499</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=7911</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2316</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=16</t>
+    <t>PlayerDetails.aspx?playerKey=12544</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=13930</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=15830</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=13930</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=20</t>
   </si>
   <si>
@@ -3772,15 +3775,18 @@
     <t>PlayerDetails.aspx?playerKey=2171</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=12544</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=10739</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=9824</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=17361</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=20144</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=81</t>
   </si>
   <si>
@@ -3790,18 +3796,15 @@
     <t>PlayerDetails.aspx?playerKey=21</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=20144</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=17944</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=9824</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=10695</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=16370</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=13261</t>
   </si>
   <si>
@@ -3811,7 +3814,7 @@
     <t>PlayerDetails.aspx?playerKey=11545</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=16370</t>
+    <t>PlayerDetails.aspx?playerKey=10550</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=187</t>
@@ -3826,19 +3829,19 @@
     <t>PlayerDetails.aspx?playerKey=14067</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=10550</t>
+    <t>PlayerDetails.aspx?playerKey=17437</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=2702</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=13782</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=17518</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=17437</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=13782</t>
+    <t>PlayerDetails.aspx?playerKey=13839</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=1368</t>
@@ -3847,42 +3850,45 @@
     <t>PlayerDetails.aspx?playerKey=3624</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=15828</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=17253</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=1407</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=8901</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=7130</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=2167</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=15828</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=13839</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=1407</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=1487</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=8901</t>
+    <t>PlayerDetails.aspx?playerKey=26871</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=2482</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=15109</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=15419</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=3895</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=1896</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=15419</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=12443</t>
   </si>
   <si>
@@ -3892,9 +3898,6 @@
     <t>PlayerDetails.aspx?playerKey=1396</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=26871</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=16634</t>
   </si>
   <si>
@@ -3904,6 +3907,9 @@
     <t>PlayerDetails.aspx?playerKey=6978</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=7703</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=2608</t>
   </si>
   <si>
@@ -3919,9 +3925,6 @@
     <t>PlayerDetails.aspx?playerKey=9165</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2482</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=10357</t>
   </si>
   <si>
@@ -3931,9 +3934,15 @@
     <t>PlayerDetails.aspx?playerKey=6527</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=174</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=903</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=31</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=2595</t>
   </si>
   <si>
@@ -3943,12 +3952,6 @@
     <t>PlayerDetails.aspx?playerKey=6081</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=31</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=174</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=1380</t>
   </si>
   <si>
@@ -3958,7 +3961,7 @@
     <t>PlayerDetails.aspx?playerKey=197</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=7703</t>
+    <t>PlayerDetails.aspx?playerKey=1748</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=13460</t>
@@ -4012,10 +4015,13 @@
     <t>PlayerDetails.aspx?playerKey=22</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=16488</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=18098</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=1748</t>
+    <t>PlayerDetails.aspx?playerKey=2204</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=144</t>
@@ -4027,9 +4033,6 @@
     <t>PlayerDetails.aspx?playerKey=17999</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2204</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=7584</t>
   </si>
   <si>
@@ -4045,9 +4048,6 @@
     <t>PlayerDetails.aspx?playerKey=2117</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=16488</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=15578</t>
   </si>
   <si>
@@ -4060,6 +4060,9 @@
     <t>PlayerDetails.aspx?playerKey=18325</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=23012</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=13388</t>
   </si>
   <si>
@@ -4078,18 +4081,21 @@
     <t>PlayerDetails.aspx?playerKey=1739</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=9583</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=189</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=17766</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=4895</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=13614</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=189</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=17766</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=26938</t>
   </si>
   <si>
@@ -4111,24 +4117,33 @@
     <t>PlayerDetails.aspx?playerKey=1687</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=23012</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=9490</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=8829</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=10554</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=11738</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=10690</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=12796</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=6982</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=1681</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=18294</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=2197</t>
   </si>
   <si>
@@ -4138,9 +4153,6 @@
     <t>PlayerDetails.aspx?playerKey=11422</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=18294</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=9713</t>
   </si>
   <si>
@@ -4150,21 +4162,12 @@
     <t>PlayerDetails.aspx?playerKey=1390</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=6982</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=2652</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=10690</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=21751</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=10554</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=26951</t>
   </si>
   <si>
@@ -4174,21 +4177,24 @@
     <t>PlayerDetails.aspx?playerKey=12162</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=48</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=13826</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=11758</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=2230</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=1083</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=1761</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2230</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=41637</t>
   </si>
   <si>
@@ -4201,12 +4207,12 @@
     <t>PlayerDetails.aspx?playerKey=15173</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=12364</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=1939</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=12364</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=7455</t>
   </si>
   <si>
@@ -4237,9 +4243,6 @@
     <t>PlayerDetails.aspx?playerKey=20201</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=48</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=10358</t>
   </si>
   <si>
@@ -4249,6 +4252,9 @@
     <t>PlayerDetails.aspx?playerKey=8983</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=9850</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=8044</t>
   </si>
   <si>
@@ -4258,7 +4264,7 @@
     <t>PlayerDetails.aspx?playerKey=16614</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=9850</t>
+    <t>PlayerDetails.aspx?playerKey=11579</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=13904</t>
@@ -4279,9 +4285,6 @@
     <t>PlayerDetails.aspx?playerKey=13836</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=11579</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=9087</t>
   </si>
   <si>
@@ -4297,6 +4300,12 @@
     <t>PlayerDetails.aspx?playerKey=2503</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=15124</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=6555</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=12388</t>
   </si>
   <si>
@@ -4306,27 +4315,21 @@
     <t>PlayerDetails.aspx?playerKey=16509</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=28012</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=4049</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=6555</t>
+    <t>PlayerDetails.aspx?playerKey=1508</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=4795</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=15124</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=28012</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=2285</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=1508</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=18282</t>
   </si>
   <si>
@@ -4345,15 +4348,12 @@
     <t>PlayerDetails.aspx?playerKey=4718</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=13322</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=5848</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=13322</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=9583</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=6565</t>
   </si>
   <si>
@@ -4369,6 +4369,9 @@
     <t>PlayerDetails.aspx?playerKey=1179</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=8847</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=7024</t>
   </si>
   <si>
@@ -4390,7 +4393,7 @@
     <t>PlayerDetails.aspx?playerKey=1046</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=8847</t>
+    <t>PlayerDetails.aspx?playerKey=27985</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=15473</t>
@@ -4426,9 +4429,6 @@
     <t>PlayerDetails.aspx?playerKey=17914</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=27985</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=2852</t>
   </si>
   <si>
@@ -4447,6 +4447,9 @@
     <t>PlayerDetails.aspx?playerKey=17086</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=21657</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=66017</t>
   </si>
   <si>
@@ -4459,7 +4462,7 @@
     <t>PlayerDetails.aspx?playerKey=11332</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=21657</t>
+    <t>PlayerDetails.aspx?playerKey=22988</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=4021</t>
@@ -4468,12 +4471,15 @@
     <t>PlayerDetails.aspx?playerKey=11923</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=4265</t>
+  </si>
+  <si>
+    <t>PlayerDetails.aspx?playerKey=2333</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=2302</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=22988</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=2201</t>
   </si>
   <si>
@@ -4510,9 +4516,6 @@
     <t>PlayerDetails.aspx?playerKey=10461</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=4265</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=21969</t>
   </si>
   <si>
@@ -4525,7 +4528,7 @@
     <t>PlayerDetails.aspx?playerKey=6026</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2333</t>
+    <t>PlayerDetails.aspx?playerKey=21648</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=2400</t>
@@ -4555,16 +4558,22 @@
     <t>PlayerDetails.aspx?playerKey=15283</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=21638</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=15609</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=10173</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=9707</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=8348</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=21638</t>
+    <t>PlayerDetails.aspx?playerKey=15321</t>
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=13243</t>
@@ -4576,12 +4585,12 @@
     <t>PlayerDetails.aspx?playerKey=16106</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=2368</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=2286</t>
   </si>
   <si>
-    <t>PlayerDetails.aspx?playerKey=2368</t>
-  </si>
-  <si>
     <t>PlayerDetails.aspx?playerKey=20233</t>
   </si>
   <si>
@@ -4609,9 +4618,15 @@
     <t>PlayerDetails.aspx?playerKey=15467</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=19051</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=12563</t>
   </si>
   <si>
+    <t>PlayerDetails.aspx?playerKey=12608</t>
+  </si>
+  <si>
     <t>PlayerDetails.aspx?playerKey=13333</t>
   </si>
   <si>
@@ -4655,21 +4670,6 @@
   </si>
   <si>
     <t>PlayerDetails.aspx?playerKey=3252</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=8216</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=6121</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=32232</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=15751</t>
-  </si>
-  <si>
-    <t>PlayerDetails.aspx?playerKey=17618</t>
   </si>
 </sst>
 </file>
@@ -6486,7 +6486,7 @@
         <v>588</v>
       </c>
       <c r="D86" t="s">
-        <v>1006</v>
+        <v>1019</v>
       </c>
       <c r="E86" t="s">
         <v>1136</v>
@@ -6503,7 +6503,7 @@
         <v>589</v>
       </c>
       <c r="D87" t="s">
-        <v>1019</v>
+        <v>1006</v>
       </c>
       <c r="E87" t="s">
         <v>1137</v>
@@ -6877,7 +6877,7 @@
         <v>611</v>
       </c>
       <c r="D109" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E109" t="s">
         <v>1159</v>
@@ -6894,7 +6894,7 @@
         <v>612</v>
       </c>
       <c r="D110" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E110" t="s">
         <v>1160</v>
@@ -6911,7 +6911,7 @@
         <v>613</v>
       </c>
       <c r="D111" t="s">
-        <v>1022</v>
+        <v>1006</v>
       </c>
       <c r="E111" t="s">
         <v>1161</v>
@@ -6928,7 +6928,7 @@
         <v>614</v>
       </c>
       <c r="D112" t="s">
-        <v>1006</v>
+        <v>1022</v>
       </c>
       <c r="E112" t="s">
         <v>1162</v>
@@ -7013,7 +7013,7 @@
         <v>619</v>
       </c>
       <c r="D117" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E117" t="s">
         <v>1167</v>
@@ -7030,7 +7030,7 @@
         <v>620</v>
       </c>
       <c r="D118" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="E118" t="s">
         <v>1168</v>
@@ -7047,7 +7047,7 @@
         <v>621</v>
       </c>
       <c r="D119" t="s">
-        <v>1021</v>
+        <v>1010</v>
       </c>
       <c r="E119" t="s">
         <v>1169</v>
@@ -7064,7 +7064,7 @@
         <v>622</v>
       </c>
       <c r="D120" t="s">
-        <v>1004</v>
+        <v>1021</v>
       </c>
       <c r="E120" t="s">
         <v>1170</v>
@@ -7081,7 +7081,7 @@
         <v>623</v>
       </c>
       <c r="D121" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E121" t="s">
         <v>1171</v>
@@ -7115,7 +7115,7 @@
         <v>625</v>
       </c>
       <c r="D123" t="s">
-        <v>1004</v>
+        <v>1019</v>
       </c>
       <c r="E123" t="s">
         <v>1173</v>
@@ -7132,7 +7132,7 @@
         <v>626</v>
       </c>
       <c r="D124" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E124" t="s">
         <v>1174</v>
@@ -7149,7 +7149,7 @@
         <v>627</v>
       </c>
       <c r="D125" t="s">
-        <v>1019</v>
+        <v>1006</v>
       </c>
       <c r="E125" t="s">
         <v>1175</v>
@@ -7217,7 +7217,7 @@
         <v>631</v>
       </c>
       <c r="D129" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E129" t="s">
         <v>1179</v>
@@ -7251,7 +7251,7 @@
         <v>633</v>
       </c>
       <c r="D131" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E131" t="s">
         <v>1181</v>
@@ -7336,7 +7336,7 @@
         <v>638</v>
       </c>
       <c r="D136" t="s">
-        <v>1005</v>
+        <v>1027</v>
       </c>
       <c r="E136" t="s">
         <v>1186</v>
@@ -7353,7 +7353,7 @@
         <v>639</v>
       </c>
       <c r="D137" t="s">
-        <v>1027</v>
+        <v>1005</v>
       </c>
       <c r="E137" t="s">
         <v>1187</v>
@@ -7370,7 +7370,7 @@
         <v>640</v>
       </c>
       <c r="D138" t="s">
-        <v>1004</v>
+        <v>1028</v>
       </c>
       <c r="E138" t="s">
         <v>1188</v>
@@ -7387,7 +7387,7 @@
         <v>641</v>
       </c>
       <c r="D139" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E139" t="s">
         <v>1189</v>
@@ -7438,7 +7438,7 @@
         <v>644</v>
       </c>
       <c r="D142" t="s">
-        <v>1028</v>
+        <v>1006</v>
       </c>
       <c r="E142" t="s">
         <v>1192</v>
@@ -7455,7 +7455,7 @@
         <v>645</v>
       </c>
       <c r="D143" t="s">
-        <v>1010</v>
+        <v>1029</v>
       </c>
       <c r="E143" t="s">
         <v>1193</v>
@@ -7472,7 +7472,7 @@
         <v>646</v>
       </c>
       <c r="D144" t="s">
-        <v>1017</v>
+        <v>1010</v>
       </c>
       <c r="E144" t="s">
         <v>1194</v>
@@ -7489,7 +7489,7 @@
         <v>647</v>
       </c>
       <c r="D145" t="s">
-        <v>1029</v>
+        <v>1017</v>
       </c>
       <c r="E145" t="s">
         <v>1195</v>
@@ -7506,7 +7506,7 @@
         <v>648</v>
       </c>
       <c r="D146" t="s">
-        <v>1006</v>
+        <v>1030</v>
       </c>
       <c r="E146" t="s">
         <v>1196</v>
@@ -7523,7 +7523,7 @@
         <v>649</v>
       </c>
       <c r="D147" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E147" t="s">
         <v>1197</v>
@@ -7540,7 +7540,7 @@
         <v>650</v>
       </c>
       <c r="D148" t="s">
-        <v>1030</v>
+        <v>1010</v>
       </c>
       <c r="E148" t="s">
         <v>1198</v>
@@ -7574,7 +7574,7 @@
         <v>652</v>
       </c>
       <c r="D150" t="s">
-        <v>1006</v>
+        <v>1024</v>
       </c>
       <c r="E150" t="s">
         <v>1200</v>
@@ -7625,7 +7625,7 @@
         <v>655</v>
       </c>
       <c r="D153" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E153" t="s">
         <v>1203</v>
@@ -7642,7 +7642,7 @@
         <v>656</v>
       </c>
       <c r="D154" t="s">
-        <v>1024</v>
+        <v>1013</v>
       </c>
       <c r="E154" t="s">
         <v>1204</v>
@@ -7710,7 +7710,7 @@
         <v>660</v>
       </c>
       <c r="D158" t="s">
-        <v>1011</v>
+        <v>1006</v>
       </c>
       <c r="E158" t="s">
         <v>1208</v>
@@ -7727,7 +7727,7 @@
         <v>661</v>
       </c>
       <c r="D159" t="s">
-        <v>1004</v>
+        <v>1011</v>
       </c>
       <c r="E159" t="s">
         <v>1209</v>
@@ -7744,7 +7744,7 @@
         <v>662</v>
       </c>
       <c r="D160" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E160" t="s">
         <v>1210</v>
@@ -7812,7 +7812,7 @@
         <v>666</v>
       </c>
       <c r="D164" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E164" t="s">
         <v>1214</v>
@@ -7931,7 +7931,7 @@
         <v>673</v>
       </c>
       <c r="D171" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="E171" t="s">
         <v>1221</v>
@@ -7948,7 +7948,7 @@
         <v>674</v>
       </c>
       <c r="D172" t="s">
-        <v>1010</v>
+        <v>1028</v>
       </c>
       <c r="E172" t="s">
         <v>1222</v>
@@ -7965,7 +7965,7 @@
         <v>675</v>
       </c>
       <c r="D173" t="s">
-        <v>1031</v>
+        <v>1010</v>
       </c>
       <c r="E173" t="s">
         <v>1223</v>
@@ -7982,7 +7982,7 @@
         <v>676</v>
       </c>
       <c r="D174" t="s">
-        <v>1006</v>
+        <v>1031</v>
       </c>
       <c r="E174" t="s">
         <v>1224</v>
@@ -8050,7 +8050,7 @@
         <v>680</v>
       </c>
       <c r="D178" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="E178" t="s">
         <v>1228</v>
@@ -8067,7 +8067,7 @@
         <v>681</v>
       </c>
       <c r="D179" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E179" t="s">
         <v>1229</v>
@@ -8220,7 +8220,7 @@
         <v>690</v>
       </c>
       <c r="D188" t="s">
-        <v>1021</v>
+        <v>1006</v>
       </c>
       <c r="E188" t="s">
         <v>1238</v>
@@ -8254,7 +8254,7 @@
         <v>692</v>
       </c>
       <c r="D190" t="s">
-        <v>1006</v>
+        <v>1021</v>
       </c>
       <c r="E190" t="s">
         <v>1240</v>
@@ -8271,7 +8271,7 @@
         <v>693</v>
       </c>
       <c r="D191" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E191" t="s">
         <v>1241</v>
@@ -8288,7 +8288,7 @@
         <v>694</v>
       </c>
       <c r="D192" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E192" t="s">
         <v>1242</v>
@@ -8305,7 +8305,7 @@
         <v>695</v>
       </c>
       <c r="D193" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="E193" t="s">
         <v>1243</v>
@@ -8356,7 +8356,7 @@
         <v>698</v>
       </c>
       <c r="D196" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E196" t="s">
         <v>1246</v>
@@ -8441,7 +8441,7 @@
         <v>703</v>
       </c>
       <c r="D201" t="s">
-        <v>1030</v>
+        <v>1006</v>
       </c>
       <c r="E201" t="s">
         <v>1251</v>
@@ -8458,7 +8458,7 @@
         <v>704</v>
       </c>
       <c r="D202" t="s">
-        <v>1006</v>
+        <v>1026</v>
       </c>
       <c r="E202" t="s">
         <v>1252</v>
@@ -8492,7 +8492,7 @@
         <v>706</v>
       </c>
       <c r="D204" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E204" t="s">
         <v>1254</v>
@@ -8509,7 +8509,7 @@
         <v>707</v>
       </c>
       <c r="D205" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E205" t="s">
         <v>1255</v>
@@ -8526,7 +8526,7 @@
         <v>708</v>
       </c>
       <c r="D206" t="s">
-        <v>1016</v>
+        <v>1008</v>
       </c>
       <c r="E206" t="s">
         <v>1256</v>
@@ -8543,7 +8543,7 @@
         <v>709</v>
       </c>
       <c r="D207" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E207" t="s">
         <v>1257</v>
@@ -8560,7 +8560,7 @@
         <v>710</v>
       </c>
       <c r="D208" t="s">
-        <v>1008</v>
+        <v>1016</v>
       </c>
       <c r="E208" t="s">
         <v>1258</v>
@@ -8577,7 +8577,7 @@
         <v>711</v>
       </c>
       <c r="D209" t="s">
-        <v>1014</v>
+        <v>1006</v>
       </c>
       <c r="E209" t="s">
         <v>1259</v>
@@ -8594,7 +8594,7 @@
         <v>712</v>
       </c>
       <c r="D210" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="E210" t="s">
         <v>1260</v>
@@ -8628,7 +8628,7 @@
         <v>714</v>
       </c>
       <c r="D212" t="s">
-        <v>1029</v>
+        <v>1007</v>
       </c>
       <c r="E212" t="s">
         <v>1262</v>
@@ -8645,7 +8645,7 @@
         <v>715</v>
       </c>
       <c r="D213" t="s">
-        <v>1004</v>
+        <v>1030</v>
       </c>
       <c r="E213" t="s">
         <v>1263</v>
@@ -8662,7 +8662,7 @@
         <v>716</v>
       </c>
       <c r="D214" t="s">
-        <v>1017</v>
+        <v>1004</v>
       </c>
       <c r="E214" t="s">
         <v>1264</v>
@@ -8679,7 +8679,7 @@
         <v>717</v>
       </c>
       <c r="D215" t="s">
-        <v>1007</v>
+        <v>1017</v>
       </c>
       <c r="E215" t="s">
         <v>1265</v>
@@ -8747,7 +8747,7 @@
         <v>721</v>
       </c>
       <c r="D219" t="s">
-        <v>1033</v>
+        <v>1006</v>
       </c>
       <c r="E219" t="s">
         <v>1269</v>
@@ -8764,7 +8764,7 @@
         <v>722</v>
       </c>
       <c r="D220" t="s">
-        <v>1006</v>
+        <v>1033</v>
       </c>
       <c r="E220" t="s">
         <v>1270</v>
@@ -8815,7 +8815,7 @@
         <v>725</v>
       </c>
       <c r="D223" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E223" t="s">
         <v>1273</v>
@@ -8832,7 +8832,7 @@
         <v>726</v>
       </c>
       <c r="D224" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E224" t="s">
         <v>1274</v>
@@ -8849,7 +8849,7 @@
         <v>727</v>
       </c>
       <c r="D225" t="s">
-        <v>1034</v>
+        <v>1006</v>
       </c>
       <c r="E225" t="s">
         <v>1275</v>
@@ -8866,7 +8866,7 @@
         <v>728</v>
       </c>
       <c r="D226" t="s">
-        <v>1006</v>
+        <v>1034</v>
       </c>
       <c r="E226" t="s">
         <v>1276</v>
@@ -8917,7 +8917,7 @@
         <v>731</v>
       </c>
       <c r="D229" t="s">
-        <v>1033</v>
+        <v>1006</v>
       </c>
       <c r="E229" t="s">
         <v>1279</v>
@@ -8951,7 +8951,7 @@
         <v>733</v>
       </c>
       <c r="D231" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E231" t="s">
         <v>1281</v>
@@ -8985,7 +8985,7 @@
         <v>735</v>
       </c>
       <c r="D233" t="s">
-        <v>1006</v>
+        <v>1033</v>
       </c>
       <c r="E233" t="s">
         <v>1283</v>
@@ -9002,7 +9002,7 @@
         <v>736</v>
       </c>
       <c r="D234" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E234" t="s">
         <v>1284</v>
@@ -9053,7 +9053,7 @@
         <v>739</v>
       </c>
       <c r="D237" t="s">
-        <v>1031</v>
+        <v>1006</v>
       </c>
       <c r="E237" t="s">
         <v>1287</v>
@@ -9087,7 +9087,7 @@
         <v>741</v>
       </c>
       <c r="D239" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E239" t="s">
         <v>1289</v>
@@ -9104,7 +9104,7 @@
         <v>742</v>
       </c>
       <c r="D240" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="E240" t="s">
         <v>1290</v>
@@ -9121,7 +9121,7 @@
         <v>743</v>
       </c>
       <c r="D241" t="s">
-        <v>1035</v>
+        <v>1010</v>
       </c>
       <c r="E241" t="s">
         <v>1291</v>
@@ -9138,7 +9138,7 @@
         <v>744</v>
       </c>
       <c r="D242" t="s">
-        <v>1006</v>
+        <v>1026</v>
       </c>
       <c r="E242" t="s">
         <v>1292</v>
@@ -9155,7 +9155,7 @@
         <v>745</v>
       </c>
       <c r="D243" t="s">
-        <v>1004</v>
+        <v>1035</v>
       </c>
       <c r="E243" t="s">
         <v>1293</v>
@@ -9189,7 +9189,7 @@
         <v>747</v>
       </c>
       <c r="D245" t="s">
-        <v>1009</v>
+        <v>1004</v>
       </c>
       <c r="E245" t="s">
         <v>1295</v>
@@ -9223,7 +9223,7 @@
         <v>749</v>
       </c>
       <c r="D247" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E247" t="s">
         <v>1297</v>
@@ -9240,7 +9240,7 @@
         <v>750</v>
       </c>
       <c r="D248" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E248" t="s">
         <v>1298</v>
@@ -9257,7 +9257,7 @@
         <v>751</v>
       </c>
       <c r="D249" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="E249" t="s">
         <v>1299</v>
@@ -9274,7 +9274,7 @@
         <v>752</v>
       </c>
       <c r="D250" t="s">
-        <v>1029</v>
+        <v>1006</v>
       </c>
       <c r="E250" t="s">
         <v>1300</v>
@@ -9308,7 +9308,7 @@
         <v>754</v>
       </c>
       <c r="D252" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E252" t="s">
         <v>1302</v>
@@ -9325,7 +9325,7 @@
         <v>755</v>
       </c>
       <c r="D253" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="E253" t="s">
         <v>1303</v>
@@ -9342,7 +9342,7 @@
         <v>756</v>
       </c>
       <c r="D254" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="E254" t="s">
         <v>1304</v>
@@ -9359,7 +9359,7 @@
         <v>757</v>
       </c>
       <c r="D255" t="s">
-        <v>1006</v>
+        <v>1036</v>
       </c>
       <c r="E255" t="s">
         <v>1305</v>
@@ -9376,7 +9376,7 @@
         <v>758</v>
       </c>
       <c r="D256" t="s">
-        <v>1021</v>
+        <v>1006</v>
       </c>
       <c r="E256" t="s">
         <v>1306</v>
@@ -9393,7 +9393,7 @@
         <v>759</v>
       </c>
       <c r="D257" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E257" t="s">
         <v>1307</v>
@@ -9410,7 +9410,7 @@
         <v>760</v>
       </c>
       <c r="D258" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E258" t="s">
         <v>1308</v>
@@ -9427,7 +9427,7 @@
         <v>761</v>
       </c>
       <c r="D259" t="s">
-        <v>1006</v>
+        <v>1021</v>
       </c>
       <c r="E259" t="s">
         <v>1309</v>
@@ -9444,7 +9444,7 @@
         <v>762</v>
       </c>
       <c r="D260" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E260" t="s">
         <v>1310</v>
@@ -9461,7 +9461,7 @@
         <v>763</v>
       </c>
       <c r="D261" t="s">
-        <v>1031</v>
+        <v>1013</v>
       </c>
       <c r="E261" t="s">
         <v>1311</v>
@@ -9478,7 +9478,7 @@
         <v>764</v>
       </c>
       <c r="D262" t="s">
-        <v>1010</v>
+        <v>1031</v>
       </c>
       <c r="E262" t="s">
         <v>1312</v>
@@ -9495,7 +9495,7 @@
         <v>765</v>
       </c>
       <c r="D263" t="s">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="E263" t="s">
         <v>1313</v>
@@ -9512,7 +9512,7 @@
         <v>766</v>
       </c>
       <c r="D264" t="s">
-        <v>1006</v>
+        <v>1019</v>
       </c>
       <c r="E264" t="s">
         <v>1314</v>
@@ -9529,7 +9529,7 @@
         <v>767</v>
       </c>
       <c r="D265" t="s">
-        <v>1035</v>
+        <v>1015</v>
       </c>
       <c r="E265" t="s">
         <v>1315</v>
@@ -9546,7 +9546,7 @@
         <v>768</v>
       </c>
       <c r="D266" t="s">
-        <v>1009</v>
+        <v>1035</v>
       </c>
       <c r="E266" t="s">
         <v>1316</v>
@@ -9563,7 +9563,7 @@
         <v>769</v>
       </c>
       <c r="D267" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E267" t="s">
         <v>1317</v>
@@ -9580,7 +9580,7 @@
         <v>770</v>
       </c>
       <c r="D268" t="s">
-        <v>1037</v>
+        <v>1006</v>
       </c>
       <c r="E268" t="s">
         <v>1318</v>
@@ -9597,7 +9597,7 @@
         <v>771</v>
       </c>
       <c r="D269" t="s">
-        <v>1004</v>
+        <v>1037</v>
       </c>
       <c r="E269" t="s">
         <v>1319</v>
@@ -9614,7 +9614,7 @@
         <v>772</v>
       </c>
       <c r="D270" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E270" t="s">
         <v>1320</v>
@@ -9631,7 +9631,7 @@
         <v>773</v>
       </c>
       <c r="D271" t="s">
-        <v>1038</v>
+        <v>1006</v>
       </c>
       <c r="E271" t="s">
         <v>1321</v>
@@ -9648,7 +9648,7 @@
         <v>774</v>
       </c>
       <c r="D272" t="s">
-        <v>1006</v>
+        <v>1038</v>
       </c>
       <c r="E272" t="s">
         <v>1322</v>
@@ -9682,7 +9682,7 @@
         <v>776</v>
       </c>
       <c r="D274" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E274" t="s">
         <v>1324</v>
@@ -9699,7 +9699,7 @@
         <v>777</v>
       </c>
       <c r="D275" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E275" t="s">
         <v>1325</v>
@@ -9716,7 +9716,7 @@
         <v>778</v>
       </c>
       <c r="D276" t="s">
-        <v>1031</v>
+        <v>1006</v>
       </c>
       <c r="E276" t="s">
         <v>1326</v>
@@ -9733,7 +9733,7 @@
         <v>779</v>
       </c>
       <c r="D277" t="s">
-        <v>1004</v>
+        <v>1031</v>
       </c>
       <c r="E277" t="s">
         <v>1327</v>
@@ -9750,7 +9750,7 @@
         <v>780</v>
       </c>
       <c r="D278" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E278" t="s">
         <v>1328</v>
@@ -9767,7 +9767,7 @@
         <v>781</v>
       </c>
       <c r="D279" t="s">
-        <v>1021</v>
+        <v>1006</v>
       </c>
       <c r="E279" t="s">
         <v>1329</v>
@@ -9784,7 +9784,7 @@
         <v>782</v>
       </c>
       <c r="D280" t="s">
-        <v>1006</v>
+        <v>1021</v>
       </c>
       <c r="E280" t="s">
         <v>1330</v>
@@ -9835,7 +9835,7 @@
         <v>785</v>
       </c>
       <c r="D283" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="E283" t="s">
         <v>1333</v>
@@ -9852,7 +9852,7 @@
         <v>786</v>
       </c>
       <c r="D284" t="s">
-        <v>1011</v>
+        <v>1006</v>
       </c>
       <c r="E284" t="s">
         <v>1334</v>
@@ -9886,7 +9886,7 @@
         <v>788</v>
       </c>
       <c r="D286" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="E286" t="s">
         <v>1336</v>
@@ -9920,7 +9920,7 @@
         <v>790</v>
       </c>
       <c r="D288" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="E288" t="s">
         <v>1338</v>
@@ -9937,7 +9937,7 @@
         <v>791</v>
       </c>
       <c r="D289" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E289" t="s">
         <v>1339</v>
@@ -9954,7 +9954,7 @@
         <v>792</v>
       </c>
       <c r="D290" t="s">
-        <v>1031</v>
+        <v>1010</v>
       </c>
       <c r="E290" t="s">
         <v>1340</v>
@@ -9971,7 +9971,7 @@
         <v>793</v>
       </c>
       <c r="D291" t="s">
-        <v>1013</v>
+        <v>1031</v>
       </c>
       <c r="E291" t="s">
         <v>1341</v>
@@ -9988,7 +9988,7 @@
         <v>794</v>
       </c>
       <c r="D292" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="E292" t="s">
         <v>1342</v>
@@ -10090,7 +10090,7 @@
         <v>800</v>
       </c>
       <c r="D298" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E298" t="s">
         <v>1348</v>
@@ -10107,7 +10107,7 @@
         <v>801</v>
       </c>
       <c r="D299" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E299" t="s">
         <v>1349</v>
@@ -10124,7 +10124,7 @@
         <v>802</v>
       </c>
       <c r="D300" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E300" t="s">
         <v>1350</v>
@@ -10158,7 +10158,7 @@
         <v>804</v>
       </c>
       <c r="D302" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E302" t="s">
         <v>1352</v>
@@ -10175,7 +10175,7 @@
         <v>805</v>
       </c>
       <c r="D303" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E303" t="s">
         <v>1353</v>
@@ -10192,7 +10192,7 @@
         <v>806</v>
       </c>
       <c r="D304" t="s">
-        <v>1030</v>
+        <v>1006</v>
       </c>
       <c r="E304" t="s">
         <v>1354</v>
@@ -10209,7 +10209,7 @@
         <v>807</v>
       </c>
       <c r="D305" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E305" t="s">
         <v>1355</v>
@@ -10260,7 +10260,7 @@
         <v>810</v>
       </c>
       <c r="D308" t="s">
-        <v>1040</v>
+        <v>1026</v>
       </c>
       <c r="E308" t="s">
         <v>1358</v>
@@ -10277,7 +10277,7 @@
         <v>811</v>
       </c>
       <c r="D309" t="s">
-        <v>1030</v>
+        <v>1013</v>
       </c>
       <c r="E309" t="s">
         <v>1359</v>
@@ -10294,7 +10294,7 @@
         <v>812</v>
       </c>
       <c r="D310" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E310" t="s">
         <v>1360</v>
@@ -10311,7 +10311,7 @@
         <v>813</v>
       </c>
       <c r="D311" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
       <c r="E311" t="s">
         <v>1361</v>
@@ -10328,7 +10328,7 @@
         <v>814</v>
       </c>
       <c r="D312" t="s">
-        <v>1017</v>
+        <v>1041</v>
       </c>
       <c r="E312" t="s">
         <v>1362</v>
@@ -10345,7 +10345,7 @@
         <v>815</v>
       </c>
       <c r="D313" t="s">
-        <v>1031</v>
+        <v>1021</v>
       </c>
       <c r="E313" t="s">
         <v>1363</v>
@@ -10362,7 +10362,7 @@
         <v>816</v>
       </c>
       <c r="D314" t="s">
-        <v>1006</v>
+        <v>1017</v>
       </c>
       <c r="E314" t="s">
         <v>1364</v>
@@ -10379,7 +10379,7 @@
         <v>817</v>
       </c>
       <c r="D315" t="s">
-        <v>1004</v>
+        <v>1031</v>
       </c>
       <c r="E315" t="s">
         <v>1365</v>
@@ -10396,7 +10396,7 @@
         <v>818</v>
       </c>
       <c r="D316" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E316" t="s">
         <v>1366</v>
@@ -10413,7 +10413,7 @@
         <v>819</v>
       </c>
       <c r="D317" t="s">
-        <v>1029</v>
+        <v>1013</v>
       </c>
       <c r="E317" t="s">
         <v>1367</v>
@@ -10430,7 +10430,7 @@
         <v>820</v>
       </c>
       <c r="D318" t="s">
-        <v>1039</v>
+        <v>1030</v>
       </c>
       <c r="E318" t="s">
         <v>1368</v>
@@ -10447,7 +10447,7 @@
         <v>821</v>
       </c>
       <c r="D319" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="E319" t="s">
         <v>1369</v>
@@ -10464,7 +10464,7 @@
         <v>822</v>
       </c>
       <c r="D320" t="s">
-        <v>1006</v>
+        <v>1039</v>
       </c>
       <c r="E320" t="s">
         <v>1370</v>
@@ -10481,7 +10481,7 @@
         <v>823</v>
       </c>
       <c r="D321" t="s">
-        <v>1042</v>
+        <v>1006</v>
       </c>
       <c r="E321" t="s">
         <v>1371</v>
@@ -10498,7 +10498,7 @@
         <v>824</v>
       </c>
       <c r="D322" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E322" t="s">
         <v>1372</v>
@@ -10515,7 +10515,7 @@
         <v>825</v>
       </c>
       <c r="D323" t="s">
-        <v>1037</v>
+        <v>1006</v>
       </c>
       <c r="E323" t="s">
         <v>1373</v>
@@ -10532,7 +10532,7 @@
         <v>826</v>
       </c>
       <c r="D324" t="s">
-        <v>1039</v>
+        <v>1006</v>
       </c>
       <c r="E324" t="s">
         <v>1374</v>
@@ -10549,7 +10549,7 @@
         <v>827</v>
       </c>
       <c r="D325" t="s">
-        <v>1009</v>
+        <v>1039</v>
       </c>
       <c r="E325" t="s">
         <v>1375</v>
@@ -10566,7 +10566,7 @@
         <v>828</v>
       </c>
       <c r="D326" t="s">
-        <v>1006</v>
+        <v>1042</v>
       </c>
       <c r="E326" t="s">
         <v>1376</v>
@@ -10600,7 +10600,7 @@
         <v>830</v>
       </c>
       <c r="D328" t="s">
-        <v>1006</v>
+        <v>1037</v>
       </c>
       <c r="E328" t="s">
         <v>1378</v>
@@ -10617,7 +10617,7 @@
         <v>831</v>
       </c>
       <c r="D329" t="s">
-        <v>1030</v>
+        <v>1009</v>
       </c>
       <c r="E329" t="s">
         <v>1379</v>
@@ -10651,7 +10651,7 @@
         <v>833</v>
       </c>
       <c r="D331" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E331" t="s">
         <v>1381</v>
@@ -10668,7 +10668,7 @@
         <v>834</v>
       </c>
       <c r="D332" t="s">
-        <v>1006</v>
+        <v>1026</v>
       </c>
       <c r="E332" t="s">
         <v>1382</v>
@@ -10685,7 +10685,7 @@
         <v>835</v>
       </c>
       <c r="D333" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="E333" t="s">
         <v>1383</v>
@@ -10702,7 +10702,7 @@
         <v>836</v>
       </c>
       <c r="D334" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E334" t="s">
         <v>1384</v>
@@ -10719,7 +10719,7 @@
         <v>837</v>
       </c>
       <c r="D335" t="s">
-        <v>1042</v>
+        <v>1006</v>
       </c>
       <c r="E335" t="s">
         <v>1385</v>
@@ -10736,7 +10736,7 @@
         <v>838</v>
       </c>
       <c r="D336" t="s">
-        <v>1011</v>
+        <v>1042</v>
       </c>
       <c r="E336" t="s">
         <v>1386</v>
@@ -10770,7 +10770,7 @@
         <v>840</v>
       </c>
       <c r="D338" t="s">
-        <v>1038</v>
+        <v>1011</v>
       </c>
       <c r="E338" t="s">
         <v>1388</v>
@@ -10787,7 +10787,7 @@
         <v>841</v>
       </c>
       <c r="D339" t="s">
-        <v>1031</v>
+        <v>1006</v>
       </c>
       <c r="E339" t="s">
         <v>1389</v>
@@ -10821,7 +10821,7 @@
         <v>843</v>
       </c>
       <c r="D341" t="s">
-        <v>1013</v>
+        <v>1038</v>
       </c>
       <c r="E341" t="s">
         <v>1391</v>
@@ -10838,7 +10838,7 @@
         <v>844</v>
       </c>
       <c r="D342" t="s">
-        <v>1016</v>
+        <v>1031</v>
       </c>
       <c r="E342" t="s">
         <v>1392</v>
@@ -10855,7 +10855,7 @@
         <v>845</v>
       </c>
       <c r="D343" t="s">
-        <v>1023</v>
+        <v>1013</v>
       </c>
       <c r="E343" t="s">
         <v>1393</v>
@@ -10872,7 +10872,7 @@
         <v>846</v>
       </c>
       <c r="D344" t="s">
-        <v>1043</v>
+        <v>1016</v>
       </c>
       <c r="E344" t="s">
         <v>1394</v>
@@ -10889,7 +10889,7 @@
         <v>847</v>
       </c>
       <c r="D345" t="s">
-        <v>1013</v>
+        <v>1023</v>
       </c>
       <c r="E345" t="s">
         <v>1395</v>
@@ -10906,7 +10906,7 @@
         <v>848</v>
       </c>
       <c r="D346" t="s">
-        <v>1004</v>
+        <v>1043</v>
       </c>
       <c r="E346" t="s">
         <v>1396</v>
@@ -10923,7 +10923,7 @@
         <v>849</v>
       </c>
       <c r="D347" t="s">
-        <v>1044</v>
+        <v>1004</v>
       </c>
       <c r="E347" t="s">
         <v>1397</v>
@@ -10957,7 +10957,7 @@
         <v>851</v>
       </c>
       <c r="D349" t="s">
-        <v>1033</v>
+        <v>1044</v>
       </c>
       <c r="E349" t="s">
         <v>1399</v>
@@ -10974,7 +10974,7 @@
         <v>852</v>
       </c>
       <c r="D350" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="E350" t="s">
         <v>1400</v>
@@ -10991,7 +10991,7 @@
         <v>853</v>
       </c>
       <c r="D351" t="s">
-        <v>1045</v>
+        <v>1033</v>
       </c>
       <c r="E351" t="s">
         <v>1401</v>
@@ -11008,7 +11008,7 @@
         <v>854</v>
       </c>
       <c r="D352" t="s">
-        <v>1031</v>
+        <v>1006</v>
       </c>
       <c r="E352" t="s">
         <v>1402</v>
@@ -11025,7 +11025,7 @@
         <v>855</v>
       </c>
       <c r="D353" t="s">
-        <v>1042</v>
+        <v>1045</v>
       </c>
       <c r="E353" t="s">
         <v>1403</v>
@@ -11042,7 +11042,7 @@
         <v>856</v>
       </c>
       <c r="D354" t="s">
-        <v>1004</v>
+        <v>1031</v>
       </c>
       <c r="E354" t="s">
         <v>1404</v>
@@ -11059,7 +11059,7 @@
         <v>857</v>
       </c>
       <c r="D355" t="s">
-        <v>1011</v>
+        <v>1042</v>
       </c>
       <c r="E355" t="s">
         <v>1405</v>
@@ -11076,7 +11076,7 @@
         <v>858</v>
       </c>
       <c r="D356" t="s">
-        <v>1033</v>
+        <v>1004</v>
       </c>
       <c r="E356" t="s">
         <v>1406</v>
@@ -11093,7 +11093,7 @@
         <v>859</v>
       </c>
       <c r="D357" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="E357" t="s">
         <v>1407</v>
@@ -11110,7 +11110,7 @@
         <v>860</v>
       </c>
       <c r="D358" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="E358" t="s">
         <v>1408</v>
@@ -11127,7 +11127,7 @@
         <v>861</v>
       </c>
       <c r="D359" t="s">
-        <v>1006</v>
+        <v>1030</v>
       </c>
       <c r="E359" t="s">
         <v>1409</v>
@@ -11144,7 +11144,7 @@
         <v>862</v>
       </c>
       <c r="D360" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E360" t="s">
         <v>1410</v>
@@ -11161,7 +11161,7 @@
         <v>863</v>
       </c>
       <c r="D361" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E361" t="s">
         <v>1411</v>
@@ -11178,7 +11178,7 @@
         <v>864</v>
       </c>
       <c r="D362" t="s">
-        <v>1037</v>
+        <v>1005</v>
       </c>
       <c r="E362" t="s">
         <v>1412</v>
@@ -11195,7 +11195,7 @@
         <v>865</v>
       </c>
       <c r="D363" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E363" t="s">
         <v>1413</v>
@@ -11212,7 +11212,7 @@
         <v>866</v>
       </c>
       <c r="D364" t="s">
-        <v>1005</v>
+        <v>1037</v>
       </c>
       <c r="E364" t="s">
         <v>1414</v>
@@ -11229,7 +11229,7 @@
         <v>867</v>
       </c>
       <c r="D365" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="E365" t="s">
         <v>1415</v>
@@ -11246,7 +11246,7 @@
         <v>868</v>
       </c>
       <c r="D366" t="s">
-        <v>1029</v>
+        <v>1039</v>
       </c>
       <c r="E366" t="s">
         <v>1416</v>
@@ -11263,7 +11263,7 @@
         <v>869</v>
       </c>
       <c r="D367" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="E367" t="s">
         <v>1417</v>
@@ -11280,7 +11280,7 @@
         <v>870</v>
       </c>
       <c r="D368" t="s">
-        <v>1021</v>
+        <v>1030</v>
       </c>
       <c r="E368" t="s">
         <v>1418</v>
@@ -11297,7 +11297,7 @@
         <v>871</v>
       </c>
       <c r="D369" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E369" t="s">
         <v>1419</v>
@@ -11314,7 +11314,7 @@
         <v>872</v>
       </c>
       <c r="D370" t="s">
-        <v>1005</v>
+        <v>1021</v>
       </c>
       <c r="E370" t="s">
         <v>1420</v>
@@ -11331,7 +11331,7 @@
         <v>873</v>
       </c>
       <c r="D371" t="s">
-        <v>1039</v>
+        <v>1006</v>
       </c>
       <c r="E371" t="s">
         <v>1421</v>
@@ -11348,7 +11348,7 @@
         <v>874</v>
       </c>
       <c r="D372" t="s">
-        <v>1010</v>
+        <v>1005</v>
       </c>
       <c r="E372" t="s">
         <v>1422</v>
@@ -11365,7 +11365,7 @@
         <v>875</v>
       </c>
       <c r="D373" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E373" t="s">
         <v>1423</v>
@@ -11433,7 +11433,7 @@
         <v>879</v>
       </c>
       <c r="D377" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E377" t="s">
         <v>1427</v>
@@ -11484,7 +11484,7 @@
         <v>882</v>
       </c>
       <c r="D380" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E380" t="s">
         <v>1430</v>
@@ -11518,7 +11518,7 @@
         <v>884</v>
       </c>
       <c r="D382" t="s">
-        <v>1046</v>
+        <v>1006</v>
       </c>
       <c r="E382" t="s">
         <v>1432</v>
@@ -11535,7 +11535,7 @@
         <v>885</v>
       </c>
       <c r="D383" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E383" t="s">
         <v>1433</v>
@@ -11552,7 +11552,7 @@
         <v>886</v>
       </c>
       <c r="D384" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E384" t="s">
         <v>1434</v>
@@ -11569,7 +11569,7 @@
         <v>887</v>
       </c>
       <c r="D385" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E385" t="s">
         <v>1435</v>
@@ -11586,7 +11586,7 @@
         <v>888</v>
       </c>
       <c r="D386" t="s">
-        <v>1006</v>
+        <v>1046</v>
       </c>
       <c r="E386" t="s">
         <v>1436</v>
@@ -11603,7 +11603,7 @@
         <v>889</v>
       </c>
       <c r="D387" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="E387" t="s">
         <v>1437</v>
@@ -11620,7 +11620,7 @@
         <v>890</v>
       </c>
       <c r="D388" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E388" t="s">
         <v>1438</v>
@@ -11637,7 +11637,7 @@
         <v>891</v>
       </c>
       <c r="D389" t="s">
-        <v>1044</v>
+        <v>1006</v>
       </c>
       <c r="E389" t="s">
         <v>1439</v>
@@ -11654,7 +11654,7 @@
         <v>892</v>
       </c>
       <c r="D390" t="s">
-        <v>1006</v>
+        <v>1044</v>
       </c>
       <c r="E390" t="s">
         <v>1440</v>
@@ -11671,7 +11671,7 @@
         <v>893</v>
       </c>
       <c r="D391" t="s">
-        <v>1035</v>
+        <v>1006</v>
       </c>
       <c r="E391" t="s">
         <v>1441</v>
@@ -11688,7 +11688,7 @@
         <v>894</v>
       </c>
       <c r="D392" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="E392" t="s">
         <v>1442</v>
@@ -11705,7 +11705,7 @@
         <v>895</v>
       </c>
       <c r="D393" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="E393" t="s">
         <v>1443</v>
@@ -11739,7 +11739,7 @@
         <v>897</v>
       </c>
       <c r="D395" t="s">
-        <v>1039</v>
+        <v>1012</v>
       </c>
       <c r="E395" t="s">
         <v>1445</v>
@@ -11756,7 +11756,7 @@
         <v>898</v>
       </c>
       <c r="D396" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="E396" t="s">
         <v>1446</v>
@@ -11841,7 +11841,7 @@
         <v>903</v>
       </c>
       <c r="D401" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="E401" t="s">
         <v>1451</v>
@@ -11858,7 +11858,7 @@
         <v>904</v>
       </c>
       <c r="D402" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="E402" t="s">
         <v>1452</v>
@@ -11875,7 +11875,7 @@
         <v>905</v>
       </c>
       <c r="D403" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="E403" t="s">
         <v>1453</v>
@@ -11892,7 +11892,7 @@
         <v>906</v>
       </c>
       <c r="D404" t="s">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="E404" t="s">
         <v>1454</v>
@@ -11909,7 +11909,7 @@
         <v>907</v>
       </c>
       <c r="D405" t="s">
-        <v>1034</v>
+        <v>1021</v>
       </c>
       <c r="E405" t="s">
         <v>1455</v>
@@ -11943,7 +11943,7 @@
         <v>909</v>
       </c>
       <c r="D407" t="s">
-        <v>1031</v>
+        <v>1034</v>
       </c>
       <c r="E407" t="s">
         <v>1457</v>
@@ -11960,7 +11960,7 @@
         <v>910</v>
       </c>
       <c r="D408" t="s">
-        <v>1015</v>
+        <v>1031</v>
       </c>
       <c r="E408" t="s">
         <v>1458</v>
@@ -11977,7 +11977,7 @@
         <v>911</v>
       </c>
       <c r="D409" t="s">
-        <v>1005</v>
+        <v>1047</v>
       </c>
       <c r="E409" t="s">
         <v>1459</v>
@@ -11994,7 +11994,7 @@
         <v>912</v>
       </c>
       <c r="D410" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E410" t="s">
         <v>1460</v>
@@ -12011,7 +12011,7 @@
         <v>913</v>
       </c>
       <c r="D411" t="s">
-        <v>1024</v>
+        <v>1006</v>
       </c>
       <c r="E411" t="s">
         <v>1461</v>
@@ -12028,7 +12028,7 @@
         <v>914</v>
       </c>
       <c r="D412" t="s">
-        <v>1004</v>
+        <v>1024</v>
       </c>
       <c r="E412" t="s">
         <v>1462</v>
@@ -12045,7 +12045,7 @@
         <v>915</v>
       </c>
       <c r="D413" t="s">
-        <v>1039</v>
+        <v>1004</v>
       </c>
       <c r="E413" t="s">
         <v>1463</v>
@@ -12062,7 +12062,7 @@
         <v>916</v>
       </c>
       <c r="D414" t="s">
-        <v>1006</v>
+        <v>1039</v>
       </c>
       <c r="E414" t="s">
         <v>1464</v>
@@ -12079,7 +12079,7 @@
         <v>917</v>
       </c>
       <c r="D415" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="E415" t="s">
         <v>1465</v>
@@ -12096,7 +12096,7 @@
         <v>918</v>
       </c>
       <c r="D416" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E416" t="s">
         <v>1466</v>
@@ -12113,7 +12113,7 @@
         <v>919</v>
       </c>
       <c r="D417" t="s">
-        <v>1011</v>
+        <v>1006</v>
       </c>
       <c r="E417" t="s">
         <v>1467</v>
@@ -12130,7 +12130,7 @@
         <v>920</v>
       </c>
       <c r="D418" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="E418" t="s">
         <v>1468</v>
@@ -12147,7 +12147,7 @@
         <v>921</v>
       </c>
       <c r="D419" t="s">
-        <v>1033</v>
+        <v>1008</v>
       </c>
       <c r="E419" t="s">
         <v>1469</v>
@@ -12164,7 +12164,7 @@
         <v>922</v>
       </c>
       <c r="D420" t="s">
-        <v>1047</v>
+        <v>1033</v>
       </c>
       <c r="E420" t="s">
         <v>1470</v>
@@ -12181,7 +12181,7 @@
         <v>923</v>
       </c>
       <c r="D421" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E421" t="s">
         <v>1471</v>
@@ -12283,7 +12283,7 @@
         <v>929</v>
       </c>
       <c r="D427" t="s">
-        <v>1004</v>
+        <v>1039</v>
       </c>
       <c r="E427" t="s">
         <v>1477</v>
@@ -12300,7 +12300,7 @@
         <v>930</v>
       </c>
       <c r="D428" t="s">
-        <v>1021</v>
+        <v>1004</v>
       </c>
       <c r="E428" t="s">
         <v>1478</v>
@@ -12317,7 +12317,7 @@
         <v>931</v>
       </c>
       <c r="D429" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="E429" t="s">
         <v>1479</v>
@@ -12334,7 +12334,7 @@
         <v>932</v>
       </c>
       <c r="D430" t="s">
-        <v>1031</v>
+        <v>1024</v>
       </c>
       <c r="E430" t="s">
         <v>1480</v>
@@ -12351,7 +12351,7 @@
         <v>933</v>
       </c>
       <c r="D431" t="s">
-        <v>1039</v>
+        <v>1031</v>
       </c>
       <c r="E431" t="s">
         <v>1481</v>
@@ -12368,7 +12368,7 @@
         <v>934</v>
       </c>
       <c r="D432" t="s">
-        <v>1006</v>
+        <v>1039</v>
       </c>
       <c r="E432" t="s">
         <v>1482</v>
@@ -12419,7 +12419,7 @@
         <v>937</v>
       </c>
       <c r="D435" t="s">
-        <v>1039</v>
+        <v>1006</v>
       </c>
       <c r="E435" t="s">
         <v>1485</v>
@@ -12436,7 +12436,7 @@
         <v>938</v>
       </c>
       <c r="D436" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="E436" t="s">
         <v>1486</v>
@@ -12453,7 +12453,7 @@
         <v>939</v>
       </c>
       <c r="D437" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E437" t="s">
         <v>1487</v>
@@ -12487,7 +12487,7 @@
         <v>941</v>
       </c>
       <c r="D439" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E439" t="s">
         <v>1489</v>
@@ -12504,7 +12504,7 @@
         <v>942</v>
       </c>
       <c r="D440" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E440" t="s">
         <v>1490</v>
@@ -12521,7 +12521,7 @@
         <v>943</v>
       </c>
       <c r="D441" t="s">
-        <v>1034</v>
+        <v>1006</v>
       </c>
       <c r="E441" t="s">
         <v>1491</v>
@@ -12538,7 +12538,7 @@
         <v>944</v>
       </c>
       <c r="D442" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E442" t="s">
         <v>1492</v>
@@ -12555,7 +12555,7 @@
         <v>945</v>
       </c>
       <c r="D443" t="s">
-        <v>1008</v>
+        <v>1034</v>
       </c>
       <c r="E443" t="s">
         <v>1493</v>
@@ -12572,7 +12572,7 @@
         <v>946</v>
       </c>
       <c r="D444" t="s">
-        <v>1048</v>
+        <v>1005</v>
       </c>
       <c r="E444" t="s">
         <v>1494</v>
@@ -12589,7 +12589,7 @@
         <v>947</v>
       </c>
       <c r="D445" t="s">
-        <v>1015</v>
+        <v>1008</v>
       </c>
       <c r="E445" t="s">
         <v>1495</v>
@@ -12606,7 +12606,7 @@
         <v>948</v>
       </c>
       <c r="D446" t="s">
-        <v>1005</v>
+        <v>1048</v>
       </c>
       <c r="E446" t="s">
         <v>1496</v>
@@ -12623,7 +12623,7 @@
         <v>949</v>
       </c>
       <c r="D447" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
       <c r="E447" t="s">
         <v>1497</v>
@@ -12640,7 +12640,7 @@
         <v>950</v>
       </c>
       <c r="D448" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E448" t="s">
         <v>1498</v>
@@ -12657,7 +12657,7 @@
         <v>951</v>
       </c>
       <c r="D449" t="s">
-        <v>1004</v>
+        <v>1024</v>
       </c>
       <c r="E449" t="s">
         <v>1499</v>
@@ -12674,7 +12674,7 @@
         <v>952</v>
       </c>
       <c r="D450" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E450" t="s">
         <v>1500</v>
@@ -12691,7 +12691,7 @@
         <v>953</v>
       </c>
       <c r="D451" t="s">
-        <v>1014</v>
+        <v>1006</v>
       </c>
       <c r="E451" t="s">
         <v>1501</v>
@@ -12708,7 +12708,7 @@
         <v>954</v>
       </c>
       <c r="D452" t="s">
-        <v>1006</v>
+        <v>1014</v>
       </c>
       <c r="E452" t="s">
         <v>1502</v>
@@ -12725,7 +12725,7 @@
         <v>955</v>
       </c>
       <c r="D453" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E453" t="s">
         <v>1503</v>
@@ -12742,7 +12742,7 @@
         <v>956</v>
       </c>
       <c r="D454" t="s">
-        <v>1009</v>
+        <v>1039</v>
       </c>
       <c r="E454" t="s">
         <v>1504</v>
@@ -12759,7 +12759,7 @@
         <v>957</v>
       </c>
       <c r="D455" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E455" t="s">
         <v>1505</v>
@@ -12776,7 +12776,7 @@
         <v>958</v>
       </c>
       <c r="D456" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="E456" t="s">
         <v>1506</v>
@@ -12793,7 +12793,7 @@
         <v>959</v>
       </c>
       <c r="D457" t="s">
-        <v>1009</v>
+        <v>1012</v>
       </c>
       <c r="E457" t="s">
         <v>1507</v>
@@ -12810,7 +12810,7 @@
         <v>960</v>
       </c>
       <c r="D458" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="E458" t="s">
         <v>1508</v>
@@ -12827,7 +12827,7 @@
         <v>961</v>
       </c>
       <c r="D459" t="s">
-        <v>1024</v>
+        <v>1011</v>
       </c>
       <c r="E459" t="s">
         <v>1509</v>
@@ -12844,7 +12844,7 @@
         <v>962</v>
       </c>
       <c r="D460" t="s">
-        <v>1006</v>
+        <v>1024</v>
       </c>
       <c r="E460" t="s">
         <v>1510</v>
@@ -12861,7 +12861,7 @@
         <v>963</v>
       </c>
       <c r="D461" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E461" t="s">
         <v>1511</v>
@@ -12878,7 +12878,7 @@
         <v>964</v>
       </c>
       <c r="D462" t="s">
-        <v>1015</v>
+        <v>1005</v>
       </c>
       <c r="E462" t="s">
         <v>1512</v>
@@ -12895,7 +12895,7 @@
         <v>965</v>
       </c>
       <c r="D463" t="s">
-        <v>1004</v>
+        <v>1015</v>
       </c>
       <c r="E463" t="s">
         <v>1513</v>
@@ -12912,7 +12912,7 @@
         <v>966</v>
       </c>
       <c r="D464" t="s">
-        <v>1049</v>
+        <v>1006</v>
       </c>
       <c r="E464" t="s">
         <v>1514</v>
@@ -12929,7 +12929,7 @@
         <v>967</v>
       </c>
       <c r="D465" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E465" t="s">
         <v>1515</v>
@@ -12946,7 +12946,7 @@
         <v>968</v>
       </c>
       <c r="D466" t="s">
-        <v>1006</v>
+        <v>1049</v>
       </c>
       <c r="E466" t="s">
         <v>1516</v>
@@ -12997,7 +12997,7 @@
         <v>971</v>
       </c>
       <c r="D469" t="s">
-        <v>1004</v>
+        <v>1039</v>
       </c>
       <c r="E469" t="s">
         <v>1519</v>
@@ -13014,7 +13014,7 @@
         <v>972</v>
       </c>
       <c r="D470" t="s">
-        <v>1050</v>
+        <v>1006</v>
       </c>
       <c r="E470" t="s">
         <v>1520</v>
@@ -13031,7 +13031,7 @@
         <v>973</v>
       </c>
       <c r="D471" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="E471" t="s">
         <v>1521</v>
@@ -13048,7 +13048,7 @@
         <v>974</v>
       </c>
       <c r="D472" t="s">
-        <v>1024</v>
+        <v>1004</v>
       </c>
       <c r="E472" t="s">
         <v>1522</v>
@@ -13065,7 +13065,7 @@
         <v>975</v>
       </c>
       <c r="D473" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="E473" t="s">
         <v>1523</v>
@@ -13082,7 +13082,7 @@
         <v>976</v>
       </c>
       <c r="D474" t="s">
-        <v>1015</v>
+        <v>1050</v>
       </c>
       <c r="E474" t="s">
         <v>1524</v>
@@ -13099,7 +13099,7 @@
         <v>977</v>
       </c>
       <c r="D475" t="s">
-        <v>1004</v>
+        <v>1024</v>
       </c>
       <c r="E475" t="s">
         <v>1525</v>
@@ -13116,7 +13116,7 @@
         <v>978</v>
       </c>
       <c r="D476" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E476" t="s">
         <v>1526</v>
@@ -13133,7 +13133,7 @@
         <v>979</v>
       </c>
       <c r="D477" t="s">
-        <v>1039</v>
+        <v>1015</v>
       </c>
       <c r="E477" t="s">
         <v>1527</v>
@@ -13150,7 +13150,7 @@
         <v>980</v>
       </c>
       <c r="D478" t="s">
-        <v>1024</v>
+        <v>1004</v>
       </c>
       <c r="E478" t="s">
         <v>1528</v>
@@ -13167,7 +13167,7 @@
         <v>981</v>
       </c>
       <c r="D479" t="s">
-        <v>1044</v>
+        <v>1006</v>
       </c>
       <c r="E479" t="s">
         <v>1529</v>
@@ -13184,7 +13184,7 @@
         <v>982</v>
       </c>
       <c r="D480" t="s">
-        <v>1006</v>
+        <v>1039</v>
       </c>
       <c r="E480" t="s">
         <v>1530</v>
@@ -13201,7 +13201,7 @@
         <v>983</v>
       </c>
       <c r="D481" t="s">
-        <v>1006</v>
+        <v>1024</v>
       </c>
       <c r="E481" t="s">
         <v>1531</v>
@@ -13218,7 +13218,7 @@
         <v>984</v>
       </c>
       <c r="D482" t="s">
-        <v>1006</v>
+        <v>1044</v>
       </c>
       <c r="E482" t="s">
         <v>1532</v>
@@ -13235,7 +13235,7 @@
         <v>985</v>
       </c>
       <c r="D483" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E483" t="s">
         <v>1533</v>
@@ -13252,7 +13252,7 @@
         <v>986</v>
       </c>
       <c r="D484" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="E484" t="s">
         <v>1534</v>
@@ -13269,7 +13269,7 @@
         <v>987</v>
       </c>
       <c r="D485" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="E485" t="s">
         <v>1535</v>
@@ -13286,7 +13286,7 @@
         <v>988</v>
       </c>
       <c r="D486" t="s">
-        <v>1024</v>
+        <v>1005</v>
       </c>
       <c r="E486" t="s">
         <v>1536</v>
@@ -13303,7 +13303,7 @@
         <v>989</v>
       </c>
       <c r="D487" t="s">
-        <v>1033</v>
+        <v>1006</v>
       </c>
       <c r="E487" t="s">
         <v>1537</v>
@@ -13320,7 +13320,7 @@
         <v>990</v>
       </c>
       <c r="D488" t="s">
-        <v>1025</v>
+        <v>1005</v>
       </c>
       <c r="E488" t="s">
         <v>1538</v>
@@ -13337,7 +13337,7 @@
         <v>991</v>
       </c>
       <c r="D489" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E489" t="s">
         <v>1539</v>
@@ -13354,7 +13354,7 @@
         <v>992</v>
       </c>
       <c r="D490" t="s">
-        <v>1047</v>
+        <v>1009</v>
       </c>
       <c r="E490" t="s">
         <v>1540</v>
@@ -13371,7 +13371,7 @@
         <v>993</v>
       </c>
       <c r="D491" t="s">
-        <v>1006</v>
+        <v>1024</v>
       </c>
       <c r="E491" t="s">
         <v>1541</v>
@@ -13388,7 +13388,7 @@
         <v>994</v>
       </c>
       <c r="D492" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="E492" t="s">
         <v>1542</v>
@@ -13405,7 +13405,7 @@
         <v>995</v>
       </c>
       <c r="D493" t="s">
-        <v>1039</v>
+        <v>1025</v>
       </c>
       <c r="E493" t="s">
         <v>1543</v>
@@ -13422,7 +13422,7 @@
         <v>996</v>
       </c>
       <c r="D494" t="s">
-        <v>1051</v>
+        <v>1005</v>
       </c>
       <c r="E494" t="s">
         <v>1544</v>
@@ -13439,7 +13439,7 @@
         <v>997</v>
       </c>
       <c r="D495" t="s">
-        <v>1021</v>
+        <v>1047</v>
       </c>
       <c r="E495" t="s">
         <v>1545</v>
@@ -13456,7 +13456,7 @@
         <v>998</v>
       </c>
       <c r="D496" t="s">
-        <v>1011</v>
+        <v>1006</v>
       </c>
       <c r="E496" t="s">
         <v>1546</v>
@@ -13473,7 +13473,7 @@
         <v>999</v>
       </c>
       <c r="D497" t="s">
-        <v>1006</v>
+        <v>1039</v>
       </c>
       <c r="E497" t="s">
         <v>1547</v>
@@ -13490,7 +13490,7 @@
         <v>1000</v>
       </c>
       <c r="D498" t="s">
-        <v>1004</v>
+        <v>1039</v>
       </c>
       <c r="E498" t="s">
         <v>1548</v>
@@ -13507,7 +13507,7 @@
         <v>1001</v>
       </c>
       <c r="D499" t="s">
-        <v>1015</v>
+        <v>1051</v>
       </c>
       <c r="E499" t="s">
         <v>1549</v>
@@ -13524,7 +13524,7 @@
         <v>1002</v>
       </c>
       <c r="D500" t="s">
-        <v>1051</v>
+        <v>1021</v>
       </c>
       <c r="E500" t="s">
         <v>1550</v>
@@ -13541,7 +13541,7 @@
         <v>1003</v>
       </c>
       <c r="D501" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="E501" t="s">
         <v>1551</v>

</xml_diff>